<commit_message>
change total number of unique protein
</commit_message>
<xml_diff>
--- a/docs/drug_protein_interaction.xlsx
+++ b/docs/drug_protein_interaction.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e342ab95cc976646/文档/GitHub/anti-coronavirus-drugs/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{E735F441-AC17-418C-8C43-FCD347EEB2FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A48ED86A-C3F7-4756-88A2-41278FE2F4CB}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="13_ncr:1_{E735F441-AC17-418C-8C43-FCD347EEB2FF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{DBA85F99-80D8-4463-9A71-76357566D29D}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{98358216-A55A-45B9-832C-B81B2FBAB045}"/>
   </bookViews>
@@ -1683,10 +1683,10 @@
     <t>https://www.drugbank.ca/drugs/DB00508</t>
   </si>
   <si>
-    <t>164 unique protein</t>
-  </si>
-  <si>
     <t xml:space="preserve">70 unique drugs </t>
+  </si>
+  <si>
+    <t>163 unique protein</t>
   </si>
 </sst>
 </file>
@@ -2063,8 +2063,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B45A011-A8C2-423A-A585-8076C2A0CE5B}">
   <dimension ref="A1:F231"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A151" workbookViewId="0">
-      <selection activeCell="D166" sqref="D166"/>
+    <sheetView tabSelected="1" topLeftCell="A220" workbookViewId="0">
+      <selection activeCell="C231" sqref="C231"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -6462,10 +6462,10 @@
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="A231" t="s">
+        <v>549</v>
+      </c>
+      <c r="C231" t="s">
         <v>550</v>
-      </c>
-      <c r="C231" t="s">
-        <v>549</v>
       </c>
     </row>
   </sheetData>

</xml_diff>